<commit_message>
Porównanie modelu z pełnymi cechami i modelu z selekcją cech. Wesołych Świąt!
</commit_message>
<xml_diff>
--- a/projekt 2 rekonstrukcja/modele_tabele.xlsx
+++ b/projekt 2 rekonstrukcja/modele_tabele.xlsx
@@ -590,24 +590,12 @@
           <t>Oversampling</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -620,24 +608,12 @@
           <t>Oversampling</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -830,24 +806,12 @@
           <t>Over+Under</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H15" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -860,24 +824,12 @@
           <t>Over+Under</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H16" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1112,24 +1064,12 @@
           <t>Oversampling</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1142,24 +1082,12 @@
           <t>Oversampling</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1352,24 +1280,12 @@
           <t>Over+Under</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H15" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1382,24 +1298,12 @@
           <t>Over+Under</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H16" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1634,24 +1538,12 @@
           <t>Oversampling</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1664,24 +1556,12 @@
           <t>Oversampling</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1862,24 +1742,12 @@
           <t>Over+Under</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H15" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1892,24 +1760,12 @@
           <t>Over+Under</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H16" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2144,24 +2000,12 @@
           <t>Oversampling</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2174,24 +2018,12 @@
           <t>Oversampling</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2384,24 +2216,12 @@
           <t>Over+Under</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H15" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2414,24 +2234,12 @@
           <t>Over+Under</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H16" t="n">
-        <v>-1</v>
-      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">

</xml_diff>